<commit_message>
Updated prediction model: change the language.
</commit_message>
<xml_diff>
--- a/Sensor Location Data.xlsx
+++ b/Sensor Location Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Satria jr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/188de0554aef43ec/CodeProjects/TIL6022-Group23-SAIL-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79544883-EC4F-47A4-9431-19F3DBCC1D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{79544883-EC4F-47A4-9431-19F3DBCC1D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F94E9826-83FA-4283-98C2-259E21AA9844}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{5ED67275-41EB-D643-BE26-4B45E0E8312C}"/>
+    <workbookView xWindow="2620" yWindow="2620" windowWidth="19200" windowHeight="11170" xr2:uid="{5ED67275-41EB-D643-BE26-4B45E0E8312C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,12 +435,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -802,20 +809,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D443C70A-0708-1944-BECF-4917B4E95506}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.4375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.3125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.4609375" customWidth="1"/>
+    <col min="2" max="2" width="27.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.69140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -832,7 +839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -849,7 +856,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -866,7 +873,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -883,7 +890,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -900,7 +907,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -917,7 +924,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -934,7 +941,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -951,7 +958,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -968,7 +975,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -985,7 +992,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1002,7 +1009,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -1019,7 +1026,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -1036,7 +1043,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -1053,7 +1060,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -1070,7 +1077,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1087,7 +1094,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -1104,7 +1111,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -1121,7 +1128,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -1138,7 +1145,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -1155,7 +1162,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -1172,7 +1179,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -1189,7 +1196,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -1206,7 +1213,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -1223,7 +1230,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>93</v>
       </c>
@@ -1240,7 +1247,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>96</v>
       </c>
@@ -1257,7 +1264,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -1271,7 +1278,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>101</v>
       </c>
@@ -1285,7 +1292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>104</v>
       </c>
@@ -1299,7 +1306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>107</v>
       </c>
@@ -1313,7 +1320,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -1327,7 +1334,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>113</v>
       </c>
@@ -1341,7 +1348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -1355,7 +1362,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>119</v>
       </c>
@@ -1369,7 +1376,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>122</v>
       </c>
@@ -1383,7 +1390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -1397,7 +1404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>128</v>
       </c>
@@ -1412,6 +1419,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>